<commit_message>
Configuração de exportação dos dados do cardápio para excel.
</commit_message>
<xml_diff>
--- a/Resources/ImpressaoCardapio.xlsx
+++ b/Resources/ImpressaoCardapio.xlsx
@@ -1,28 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\movtech\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\movtech\Desktop\WorkSpace\TCC\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445A6E2F-6D55-483D-BB7A-B927F1580A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157E7049-8F49-4EB0-8A21-0D7C3621B1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="5550" windowWidth="28800" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Impressao" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Impressao!$A$1:$R$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Impressao!$A$1:$R$17</definedName>
     <definedName name="atendente">Impressao!#REF!</definedName>
     <definedName name="cepCidade">Impressao!#REF!</definedName>
     <definedName name="cnpjEmpresa">Impressao!$I$1</definedName>
     <definedName name="codOrcamento">Impressao!#REF!</definedName>
     <definedName name="codPedido">Impressao!#REF!</definedName>
+    <definedName name="colAlimento">Impressao!$C$8</definedName>
+    <definedName name="colItemRef">Impressao!$A$9</definedName>
+    <definedName name="colMedCaseira">Impressao!$I$8</definedName>
+    <definedName name="colObserv">Impressao!$N$8</definedName>
+    <definedName name="colRefeicao">Impressao!$A$8</definedName>
     <definedName name="condicaoPagto">Impressao!#REF!</definedName>
+    <definedName name="dataConsulta">Impressao!$B$5</definedName>
     <definedName name="dataEmissao">Impressao!#REF!</definedName>
     <definedName name="dataValidade">Impressao!#REF!</definedName>
     <definedName name="enderecoCliente">Impressao!#REF!</definedName>
@@ -49,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Paciente:</t>
   </si>
@@ -68,15 +74,19 @@
   <si>
     <t>Medida Caseira</t>
   </si>
+  <si>
+    <t>Data Consulta:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;????_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -206,89 +216,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -630,65 +635,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A3" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="4" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="2.5703125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="2.28515625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="2.28515625" style="4" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="3" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="2.88671875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="2.5546875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="2.33203125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="2.33203125" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-    </row>
-    <row r="2" spans="1:18" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+    <row r="1" spans="1:18" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+    </row>
+    <row r="2" spans="1:18" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
-      <c r="I2" s="17"/>
+      <c r="I2" s="5"/>
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
@@ -699,315 +704,338 @@
       <c r="Q2"/>
       <c r="R2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
       <c r="P3"/>
       <c r="Q3"/>
       <c r="R3"/>
     </row>
-    <row r="4" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-    </row>
-    <row r="5" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-    </row>
-    <row r="6" spans="1:18" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-    </row>
-    <row r="7" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="31" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+    </row>
+    <row r="7" spans="1:18" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+    </row>
+    <row r="8" spans="1:18" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="31" t="s">
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="24" t="s">
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="O7" s="26"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="25"/>
-    </row>
-    <row r="8" spans="1:18" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="1"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="11"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="9"/>
+    </row>
+    <row r="9" spans="1:18" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="27"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="25"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="I8:M8"/>
-    <mergeCell ref="I7:M7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:R16"/>
+  <mergeCells count="16">
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="E15:R17"/>
     <mergeCell ref="I1:R1"/>
-    <mergeCell ref="E6:R6"/>
-    <mergeCell ref="A5:R5"/>
-    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="E7:R7"/>
+    <mergeCell ref="A6:R6"/>
+    <mergeCell ref="P11:Q11"/>
     <mergeCell ref="B3:O3"/>
     <mergeCell ref="B4:O4"/>
-    <mergeCell ref="N8:R8"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="N8:Q8"/>
   </mergeCells>
   <pageMargins left="0.16213235294117648" right="0.62450980392156863" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="49" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>